<commit_message>
Corrections from Aurélie T.
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/check_protocol/STEC poumon DCA.xlsx
+++ b/Plancheck/plancheck_data/check_protocol/STEC poumon DCA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -442,18 +442,6 @@
     <t>PlexusGche</t>
   </si>
   <si>
-    <t>ITV 3ph</t>
-  </si>
-  <si>
-    <t>ITV 6ph</t>
-  </si>
-  <si>
-    <t>PTV 3ph</t>
-  </si>
-  <si>
-    <t>PTV 6ph</t>
-  </si>
-  <si>
     <t>Poumons-ITV</t>
   </si>
   <si>
@@ -500,6 +488,18 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>ITV3ph</t>
+  </si>
+  <si>
+    <t>ITV6ph</t>
+  </si>
+  <si>
+    <t>PTV3ph</t>
+  </si>
+  <si>
+    <t>PTV6ph</t>
   </si>
 </sst>
 </file>
@@ -1970,10 +1970,10 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C32" s="27"/>
       <c r="D32" s="27"/>
@@ -2021,10 +2021,10 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C35" s="27"/>
       <c r="D35" s="27"/>
@@ -2072,10 +2072,10 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C38" s="27"/>
       <c r="D38" s="27"/>
@@ -2089,10 +2089,10 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C39" s="27"/>
       <c r="D39" s="27"/>
@@ -2109,7 +2109,7 @@
         <v>78</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="27"/>
@@ -2313,8 +2313,8 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2497,22 +2497,22 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2550,7 +2550,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
@@ -2559,7 +2559,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12" t="s">
@@ -2587,7 +2587,7 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>
@@ -2718,17 +2718,17 @@
         <v>121</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
@@ -2738,10 +2738,10 @@
         <v>136</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D4" s="6"/>
     </row>
@@ -2786,7 +2786,7 @@
         <v>135</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
@@ -2796,7 +2796,7 @@
         <v>119</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>

</xml_diff>